<commit_message>
add CQ4-3 (for recipe video)
</commit_message>
<xml_diff>
--- a/requirements/requirements-CQs.xlsx
+++ b/requirements/requirements-CQs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanar\Desktop\Work\IDA\Projects\GitLab\fuskg\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CF3D71-3070-4D77-99C1-1622E83F89EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579A73EE-6E4B-40C7-9BA1-22B5F5DF34C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>CQ- ID</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>Which are the activities of category C that consume at least 200 kcal?</t>
+  </si>
+  <si>
+    <t>Where is it possible to find a video showing how to prepare recipe Z?</t>
+  </si>
+  <si>
+    <t>CQ4-3</t>
   </si>
 </sst>
 </file>
@@ -778,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,31 +972,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>43</v>
-      </c>
+    <row r="19" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -998,10 +1004,10 @@
         <v>8</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1009,37 +1015,37 @@
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C24" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>52</v>
-      </c>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1047,10 +1053,10 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1058,38 +1064,38 @@
         <v>9</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="K29" s="12"/>
-    </row>
-    <row r="30" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>59</v>
-      </c>
+    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="K30" s="12"/>
     </row>
     <row r="31" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1097,9 +1103,20 @@
         <v>10</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="10" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C33" s="11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1111,6 +1128,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="6a60e2f5-e663-45b7-9051-ee3c8521a2cc">
@@ -1119,15 +1145,6 @@
     <TaxCatchAll xmlns="49e364f8-bd3b-41c6-8911-b59b97be73e9" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1340,20 +1357,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21152A3F-6C8B-486B-9DE4-8A74F4F4EEDA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73B3A5A3-46D0-40F0-8946-BD14A21BBDF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="6a60e2f5-e663-45b7-9051-ee3c8521a2cc"/>
     <ds:schemaRef ds:uri="49e364f8-bd3b-41c6-8911-b59b97be73e9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21152A3F-6C8B-486B-9DE4-8A74F4F4EEDA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>